<commit_message>
AddAccount functionality is added
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -27,31 +27,31 @@
     <t>Industry Type</t>
   </si>
   <si>
+    <t>Government</t>
+  </si>
+  <si>
+    <t>Client Address</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>Delivery Managers</t>
+  </si>
+  <si>
+    <t>Srilatha Nerella</t>
+  </si>
+  <si>
+    <t>Industry type</t>
+  </si>
+  <si>
+    <t>Retail</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
     <t>HealthCare</t>
-  </si>
-  <si>
-    <t>Client Address</t>
-  </si>
-  <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Delivery Managers</t>
-  </si>
-  <si>
-    <t>Srilatha Nerella</t>
-  </si>
-  <si>
-    <t>Industry type</t>
-  </si>
-  <si>
-    <t>Retail</t>
-  </si>
-  <si>
-    <t>Finance</t>
-  </si>
-  <si>
-    <t>Government</t>
   </si>
   <si>
     <t>Insurance</t>
@@ -62,10 +62,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -84,6 +84,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -91,24 +106,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -123,7 +122,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -137,8 +136,24 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -148,28 +163,6 @@
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -183,14 +176,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -200,29 +185,44 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -243,187 +243,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,28 +437,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -487,11 +476,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -505,17 +500,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -534,153 +523,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="4" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1016,7 +1016,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
@@ -1101,13 +1101,13 @@
     <row r="3" spans="1:2">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">

</xml_diff>

<commit_message>
AddAccount functionality is successfully completed
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,11 +4,12 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9467"/>
+    <workbookView windowWidth="16968" windowHeight="5507"/>
   </bookViews>
   <sheets>
     <sheet name="AddAccount" sheetId="1" r:id="rId1"/>
     <sheet name="Dropdown Data" sheetId="2" r:id="rId2"/>
+    <sheet name="AddEmployee" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:G10"/>
@@ -39,7 +40,7 @@
     <t>Delivery Managers</t>
   </si>
   <si>
-    <t>Srilatha Nerella</t>
+    <t>Srilatha Nerella,Gopal Rao Pandula</t>
   </si>
   <si>
     <t>Industry type</t>
@@ -62,9 +63,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
@@ -84,8 +85,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -99,8 +124,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -122,25 +169,40 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -152,77 +214,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -249,31 +250,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -285,145 +418,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -434,6 +435,15 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -452,11 +462,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -476,17 +492,22 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -496,15 +517,6 @@
       <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -523,23 +535,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -548,139 +552,136 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1016,13 +1017,13 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
+    <col min="2" max="2" width="29.5555555555556" customWidth="1"/>
     <col min="52" max="52" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1128,4 +1129,20 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update Account functionality is successfully completed
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
   <si>
     <t>Account Name</t>
   </si>
@@ -38,6 +38,12 @@
   </si>
   <si>
     <t>Delivery Managers</t>
+  </si>
+  <si>
+    <t>Aakash deep varma,Abdul Mazeed Mahammad</t>
+  </si>
+  <si>
+    <t>Remove Delivery Managers</t>
   </si>
   <si>
     <t>Srilatha Nerella,Gopal Rao Pandula</t>
@@ -64,9 +70,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -85,6 +91,65 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <i/>
       <sz val="11"/>
       <color rgb="FF7F7F7F"/>
@@ -98,6 +163,21 @@
       <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -117,8 +197,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,81 +214,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -244,181 +250,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,24 +446,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -473,6 +466,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -494,11 +496,24 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
       <top style="thin">
-        <color theme="4"/>
+        <color rgb="FFB2B2B2"/>
       </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -508,15 +523,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -540,148 +546,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="30" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1014,16 +1020,16 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="17.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="29.5555555555556" customWidth="1"/>
+    <col min="1" max="1" width="25.5555555555556" customWidth="1"/>
+    <col min="2" max="2" width="43.2222222222222" customWidth="1"/>
     <col min="52" max="52" width="12" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1057,6 +1063,14 @@
       </c>
       <c r="B4" t="s">
         <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1087,22 +1101,22 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1114,7 +1128,7 @@
     <row r="5" spans="1:2">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
AddDomain functionality is completed
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,12 +4,15 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16968" windowHeight="5507"/>
+    <workbookView windowWidth="22943" windowHeight="9875"/>
   </bookViews>
   <sheets>
     <sheet name="AddAccount" sheetId="1" r:id="rId1"/>
-    <sheet name="Dropdown Data" sheetId="2" r:id="rId2"/>
-    <sheet name="AddEmployee" sheetId="3" r:id="rId3"/>
+    <sheet name="UpdateAccount" sheetId="6" r:id="rId2"/>
+    <sheet name="Dropdown Data" sheetId="2" r:id="rId3"/>
+    <sheet name="AddEmployee" sheetId="3" r:id="rId4"/>
+    <sheet name="AddDomain" sheetId="4" r:id="rId5"/>
+    <sheet name="UpdateDomain" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:G10"/>
@@ -17,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22">
   <si>
     <t>Account Name</t>
   </si>
@@ -40,15 +43,15 @@
     <t>Delivery Managers</t>
   </si>
   <si>
+    <t>Srilatha Nerella,Gopal Rao Pandula</t>
+  </si>
+  <si>
     <t>Aakash deep varma,Abdul Mazeed Mahammad</t>
   </si>
   <si>
     <t>Remove Delivery Managers</t>
   </si>
   <si>
-    <t>Srilatha Nerella,Gopal Rao Pandula</t>
-  </si>
-  <si>
     <t>Industry type</t>
   </si>
   <si>
@@ -62,6 +65,27 @@
   </si>
   <si>
     <t>Insurance</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Domain Name</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Delivery Lead</t>
+  </si>
+  <si>
+    <t>Adinarayana Addanki,Murali Krishna Gumpalli</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arun Kumar Guduri,Chozhan Dharmapuri Madhesh </t>
+  </si>
+  <si>
+    <t>Remove Delivery Lead</t>
   </si>
 </sst>
 </file>
@@ -70,9 +94,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -92,14 +116,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -107,21 +131,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -137,16 +147,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -167,17 +170,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -197,7 +206,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -213,6 +221,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -222,14 +254,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -250,6 +274,144 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -262,7 +424,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -274,163 +448,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -444,12 +468,25 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
+      <top/>
+      <bottom style="medium">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -474,22 +511,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -497,8 +519,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -520,9 +542,11 @@
     <border>
       <left/>
       <right/>
-      <top/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
       <bottom style="double">
-        <color rgb="FFFF8001"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -546,148 +570,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="22" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -695,11 +719,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1020,13 +1044,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="1" width="25.5555555555556" customWidth="1"/>
     <col min="2" max="2" width="43.2222222222222" customWidth="1"/>
@@ -1034,7 +1058,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1042,7 +1066,7 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
@@ -1050,7 +1074,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
@@ -1058,19 +1082,11 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1090,6 +1106,72 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="4" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="26.4444444444444" customWidth="1"/>
+    <col min="2" max="2" width="43.2222222222222" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+      <formula1>'Dropdown Data'!$B$1:$B$5</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
@@ -1100,7 +1182,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B1" t="s">
@@ -1108,25 +1190,25 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1"/>
+      <c r="A2" s="2"/>
       <c r="B2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="1"/>
+      <c r="A3" s="2"/>
       <c r="B3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="1"/>
+      <c r="A4" s="2"/>
       <c r="B4" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="1"/>
+      <c r="A5" s="2"/>
       <c r="B5" t="s">
         <v>14</v>
       </c>
@@ -1145,7 +1227,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1"/>
@@ -1159,4 +1241,102 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="2" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="13.7777777777778" customWidth="1"/>
+    <col min="2" max="2" width="41.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="20.8888888888889" customWidth="1"/>
+    <col min="2" max="2" width="41.7777777777778" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Project error messages validations completed
</commit_message>
<xml_diff>
--- a/src/main/resources/TestData.xlsx
+++ b/src/main/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22943" windowHeight="9875" activeTab="7"/>
+    <workbookView windowWidth="22943" windowHeight="9875" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="AddAccount" sheetId="1" r:id="rId1"/>
@@ -15,6 +15,7 @@
     <sheet name="UpdateDomain" sheetId="5" r:id="rId6"/>
     <sheet name="AddProject" sheetId="7" r:id="rId7"/>
     <sheet name="UpdateProject" sheetId="8" r:id="rId8"/>
+    <sheet name="AddTeamMate" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
   <oleSize ref="A1:G10"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51">
   <si>
     <t>Account Name</t>
   </si>
@@ -84,6 +85,51 @@
     <t>Proposed</t>
   </si>
   <si>
+    <t>Assigned Role</t>
+  </si>
+  <si>
+    <t>Lead</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Shift</t>
+  </si>
+  <si>
+    <t>Shift 1(9:00 AM - 6:00 PM)</t>
+  </si>
+  <si>
+    <t>Shift 2(2:00 PM - 11:00 PM)</t>
+  </si>
+  <si>
+    <t>Shift 3(10:00 PM - 6:00 AM)</t>
+  </si>
+  <si>
+    <t>Shift 4(7:30 AM - 3:30 PM)</t>
+  </si>
+  <si>
+    <t>Shift 5(11:30 AM - 7:30 PM)</t>
+  </si>
+  <si>
+    <t>Billability Status</t>
+  </si>
+  <si>
+    <t>Billable</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Non-Billable</t>
+  </si>
+  <si>
+    <t>Reserved</t>
+  </si>
+  <si>
+    <t>Trainee</t>
+  </si>
+  <si>
     <t>Account</t>
   </si>
   <si>
@@ -120,19 +166,29 @@
     <t>Project End Date</t>
   </si>
   <si>
-    <t>2018-9-30</t>
+    <t>Select a Employee</t>
+  </si>
+  <si>
+    <t>Nitin Lavania</t>
+  </si>
+  <si>
+    <t>Start Date</t>
+  </si>
+  <si>
+    <t>End Date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="176" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="181" formatCode="[$-14009]dd/mm/yyyy;@"/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -159,7 +215,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -180,8 +251,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,44 +308,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -264,6 +322,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color theme="1"/>
@@ -272,9 +337,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -286,14 +350,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="34">
     <fill>
@@ -316,43 +372,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -364,133 +546,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -501,39 +557,6 @@
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -555,8 +578,56 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -586,27 +657,12 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -624,134 +680,134 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="18" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="29" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -761,8 +817,11 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1211,16 +1270,16 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:B25"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.5555555555556" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="1" max="1" width="18.6851851851852" customWidth="1"/>
+    <col min="2" max="2" width="24.5555555555556" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1281,10 +1340,91 @@
         <v>19</v>
       </c>
     </row>
+    <row r="12" spans="1:2">
+      <c r="A12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="A13" s="5"/>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="A16" s="5"/>
+      <c r="B16" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
+      <c r="A17" s="5"/>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18" s="5"/>
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="A19" s="5"/>
+      <c r="B19" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B21" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="A22" s="5"/>
+      <c r="B22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="A23" s="5"/>
+      <c r="B23" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
+      <c r="A24" s="5"/>
+      <c r="B24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
+      <c r="A25" s="5"/>
+      <c r="B25" t="s">
+        <v>34</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="5">
     <mergeCell ref="A1:A5"/>
     <mergeCell ref="A7:A10"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A15:A19"/>
+    <mergeCell ref="A21:A25"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4 B7">
@@ -1332,7 +1472,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1340,10 +1480,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1351,7 +1491,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1517,7 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
@@ -1385,10 +1525,10 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="B2" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1396,7 +1536,7 @@
         <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1404,7 +1544,7 @@
         <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1419,7 +1559,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1:B7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="1"/>
@@ -1430,15 +1570,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1446,18 +1586,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1470,18 +1610,18 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B6" s="2">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3">
         <v>43344</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="3">
+        <v>43373</v>
       </c>
     </row>
   </sheetData>
@@ -1500,8 +1640,8 @@
   <sheetPr/>
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="6" outlineLevelCol="1"/>
@@ -1512,15 +1652,15 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="B1" t="s">
-        <v>26</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="B2" t="s">
         <v>1</v>
@@ -1528,18 +1668,18 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>42</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1552,7 +1692,7 @@
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="B6" s="2">
         <v>43344</v>
@@ -1560,10 +1700,10 @@
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="B7" s="2">
+        <v>43373</v>
       </c>
     </row>
   </sheetData>
@@ -1575,4 +1715,58 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.88888888888889" defaultRowHeight="14.4" outlineLevelRow="5" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="17.2222222222222" customWidth="1"/>
+    <col min="2" max="2" width="20.6666666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>